<commit_message>
Referencias mista, relativa e absluta
</commit_message>
<xml_diff>
--- a/2-Basico/Funções+Básicas01.xlsx
+++ b/2-Basico/Funções+Básicas01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Curso_Excel_BI_Udemy\2-Basico\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{096FF57E-C21E-4698-8F8D-CC79483E2024}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{132E6E59-1B39-4748-9732-17EC992EC56D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showSheetTabs="0" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="959" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView showSheetTabs="0" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="959" firstSheet="6" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="14" r:id="rId1"/>
@@ -1015,7 +1015,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="909" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="431">
   <si>
     <t>Total de mercadorias vendidas</t>
   </si>
@@ -2367,6 +2367,15 @@
   </si>
   <si>
     <t>(ALTOSOMA)</t>
+  </si>
+  <si>
+    <t>Idade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Atual </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data de nascimento  </t>
   </si>
 </sst>
 </file>
@@ -3647,7 +3656,7 @@
     <xf numFmtId="9" fontId="39" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="41" fillId="7" borderId="36" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="317">
+  <cellXfs count="318">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4389,6 +4398,7 @@
     </xf>
     <xf numFmtId="168" fontId="72" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="27">
     <cellStyle name="20% - Ênfase1" xfId="1" builtinId="30"/>
@@ -7410,8 +7420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10329,7 +10339,7 @@
       </c>
       <c r="G5" s="57">
         <f ca="1">TODAY()</f>
-        <v>46075</v>
+        <v>46076</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -10351,7 +10361,7 @@
       </c>
       <c r="G6" s="312">
         <f ca="1">TODAY()+30</f>
-        <v>46105</v>
+        <v>46106</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -10373,7 +10383,7 @@
       </c>
       <c r="G7" s="313">
         <f ca="1">NOW()</f>
-        <v>46075.690404629633</v>
+        <v>46076.527179861114</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -13471,9 +13481,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A2:D16"/>
+  <dimension ref="A2:G16"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -13481,9 +13493,11 @@
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:7">
       <c r="A2" s="224" t="s">
         <v>167</v>
       </c>
@@ -13491,13 +13505,13 @@
       <c r="C2" s="224"/>
       <c r="D2" s="224"/>
     </row>
-    <row r="3" spans="1:4" ht="8.25" customHeight="1">
+    <row r="3" spans="1:7" ht="8.25" customHeight="1">
       <c r="A3" s="225"/>
       <c r="B3" s="225"/>
       <c r="C3" s="225"/>
       <c r="D3" s="225"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:7">
       <c r="A4" s="21" t="s">
         <v>169</v>
       </c>
@@ -13511,7 +13525,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:7">
       <c r="A5" s="20" t="s">
         <v>172</v>
       </c>
@@ -13521,23 +13535,35 @@
       <c r="C5" s="34">
         <v>0.1</v>
       </c>
-      <c r="D5" s="55"/>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="D5" s="55">
+        <f>B5*C5</f>
+        <v>5</v>
+      </c>
+      <c r="F5" s="317">
+        <f>B5*(1+C5)</f>
+        <v>55.000000000000007</v>
+      </c>
+      <c r="G5" s="317">
+        <f>B5*110%</f>
+        <v>55.000000000000007</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="224" t="s">
         <v>167</v>
       </c>
       <c r="B8" s="224"/>
       <c r="C8" s="224"/>
       <c r="D8" s="224"/>
-    </row>
-    <row r="9" spans="1:4" ht="9" customHeight="1">
+      <c r="F8" s="310"/>
+    </row>
+    <row r="9" spans="1:7" ht="9" customHeight="1">
       <c r="A9" s="226"/>
       <c r="B9" s="227"/>
       <c r="C9" s="227"/>
       <c r="D9" s="228"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:7">
       <c r="A10" s="20" t="s">
         <v>174</v>
       </c>
@@ -13551,7 +13577,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:7">
       <c r="A11" s="20" t="s">
         <v>177</v>
       </c>
@@ -13561,38 +13587,77 @@
       <c r="C11" s="34">
         <v>0.08</v>
       </c>
-      <c r="D11" s="55"/>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="D11" s="55">
+        <f>B11-B11*C11</f>
+        <v>920</v>
+      </c>
+      <c r="F11" s="317">
+        <f>B11*(1-C11)</f>
+        <v>920</v>
+      </c>
+      <c r="G11" s="317">
+        <f>B11*92%</f>
+        <v>920</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="224" t="s">
         <v>181</v>
       </c>
       <c r="B13" s="224"/>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="F13" s="224" t="s">
+        <v>428</v>
+      </c>
+      <c r="G13" s="224"/>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="20" t="s">
         <v>178</v>
       </c>
       <c r="B14" s="33">
         <v>40964</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="F14" s="20" t="s">
+        <v>429</v>
+      </c>
+      <c r="G14" s="33">
+        <f ca="1">TODAY()</f>
+        <v>46076</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" s="20" t="s">
         <v>179</v>
       </c>
       <c r="B15" s="33">
         <v>40949</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="F15" s="20" t="s">
+        <v>430</v>
+      </c>
+      <c r="G15" s="33">
+        <v>40949</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" s="20" t="s">
         <v>180</v>
       </c>
-      <c r="B16" s="32"/>
+      <c r="B16" s="32">
+        <f>B14-B15</f>
+        <v>15</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>428</v>
+      </c>
+      <c r="G16" s="32" t="str">
+        <f ca="1">DATEDIF(G15,G14, "Y")&amp; " anos"</f>
+        <v>14 anos</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="F13:G13"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A8:D8"/>
     <mergeCell ref="A13:B13"/>

</xml_diff>